<commit_message>
24 apr cdc update
</commit_message>
<xml_diff>
--- a/data/CDC_data_new.xlsx
+++ b/data/CDC_data_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\COVID-19_epi_info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC8DB55F-DF82-430F-BD97-1359E322A9EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86037D3-34D5-43E6-AB6E-458C33502CEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="210" windowWidth="15615" windowHeight="10305" xr2:uid="{54C3C07C-4DC6-4390-B72E-2F618362C669}"/>
+    <workbookView xWindow="1980" yWindow="330" windowWidth="15615" windowHeight="9600" xr2:uid="{54C3C07C-4DC6-4390-B72E-2F618362C669}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -77,7 +77,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD0955C-1409-48F0-89A7-0CBF4F20C7A8}">
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:B94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -742,7 +742,7 @@
         <v>43893</v>
       </c>
       <c r="B43">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -766,7 +766,7 @@
         <v>43896</v>
       </c>
       <c r="B46">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -774,7 +774,7 @@
         <v>43897</v>
       </c>
       <c r="B47">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
         <v>43898</v>
       </c>
       <c r="B48">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
         <v>43905</v>
       </c>
       <c r="B55">
-        <v>3471</v>
+        <v>3487</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -854,7 +854,7 @@
         <v>43907</v>
       </c>
       <c r="B57">
-        <v>7023</v>
+        <v>7038</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -894,7 +894,7 @@
         <v>43912</v>
       </c>
       <c r="B62">
-        <v>22404</v>
+        <v>33404</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -902,7 +902,7 @@
         <v>43913</v>
       </c>
       <c r="B63">
-        <v>44338</v>
+        <v>44183</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -990,7 +990,7 @@
         <v>43924</v>
       </c>
       <c r="B74">
-        <v>258098</v>
+        <v>277205</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -998,7 +998,7 @@
         <v>43925</v>
       </c>
       <c r="B75">
-        <v>267436</v>
+        <v>304826</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1022,7 +1022,7 @@
         <v>43928</v>
       </c>
       <c r="B78">
-        <v>395926</v>
+        <v>395011</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1127,6 +1127,30 @@
       </c>
       <c r="B91">
         <v>776093</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>43942</v>
+      </c>
+      <c r="B92">
+        <v>802583</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>43943</v>
+      </c>
+      <c r="B93">
+        <v>828441</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>43944</v>
+      </c>
+      <c r="B94">
+        <v>865585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updata for cdc data and results both cdc and who
</commit_message>
<xml_diff>
--- a/data/CDC_data_new.xlsx
+++ b/data/CDC_data_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\COVID-19_epi_info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86037D3-34D5-43E6-AB6E-458C33502CEC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6294D4A-E350-443E-87E1-7B1AD8147AB9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="330" windowWidth="15615" windowHeight="9600" xr2:uid="{54C3C07C-4DC6-4390-B72E-2F618362C669}"/>
+    <workbookView xWindow="2475" yWindow="1005" windowWidth="21945" windowHeight="8745" xr2:uid="{54C3C07C-4DC6-4390-B72E-2F618362C669}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -392,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD0955C-1409-48F0-89A7-0CBF4F20C7A8}">
-  <dimension ref="A1:B94"/>
+  <dimension ref="A1:B97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -742,7 +742,7 @@
         <v>43893</v>
       </c>
       <c r="B43">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -766,7 +766,7 @@
         <v>43896</v>
       </c>
       <c r="B46">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -774,7 +774,7 @@
         <v>43897</v>
       </c>
       <c r="B47">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
         <v>43898</v>
       </c>
       <c r="B48">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
         <v>43905</v>
       </c>
       <c r="B55">
-        <v>3487</v>
+        <v>3471</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -854,7 +854,7 @@
         <v>43907</v>
       </c>
       <c r="B57">
-        <v>7038</v>
+        <v>7023</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -902,7 +902,7 @@
         <v>43913</v>
       </c>
       <c r="B63">
-        <v>44183</v>
+        <v>44338</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -990,7 +990,7 @@
         <v>43924</v>
       </c>
       <c r="B74">
-        <v>277205</v>
+        <v>258098</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -998,7 +998,7 @@
         <v>43925</v>
       </c>
       <c r="B75">
-        <v>304826</v>
+        <v>267436</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1022,7 +1022,7 @@
         <v>43928</v>
       </c>
       <c r="B78">
-        <v>395011</v>
+        <v>395926</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1151,6 +1151,30 @@
       </c>
       <c r="B94">
         <v>865585</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>43945</v>
+      </c>
+      <c r="B95">
+        <v>895766</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>43946</v>
+      </c>
+      <c r="B96">
+        <v>928619</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>43947</v>
+      </c>
+      <c r="B97">
+        <v>957875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CDC 29 Apr data
</commit_message>
<xml_diff>
--- a/data/CDC_data_new.xlsx
+++ b/data/CDC_data_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauernd\Documents\R\workspace\COVID-19_epi_info\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6294D4A-E350-443E-87E1-7B1AD8147AB9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640912D9-9241-45E5-91CF-08D1B7192F7D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="1005" windowWidth="21945" windowHeight="8745" xr2:uid="{54C3C07C-4DC6-4390-B72E-2F618362C669}"/>
+    <workbookView xWindow="4020" yWindow="1050" windowWidth="15615" windowHeight="9600" xr2:uid="{54C3C07C-4DC6-4390-B72E-2F618362C669}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -392,9 +392,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD0955C-1409-48F0-89A7-0CBF4F20C7A8}">
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:B98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1174,7 +1176,15 @@
         <v>43947</v>
       </c>
       <c r="B97">
-        <v>957875</v>
+        <v>962491</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>43948</v>
+      </c>
+      <c r="B98">
+        <v>981246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>